<commit_message>
correção 1 - relatorio final
</commit_message>
<xml_diff>
--- a/dados/Contagem de Pantas Atacadas/acont.xlsx
+++ b/dados/Contagem de Pantas Atacadas/acont.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documents\Data Science\FitoData\Projetos\Daniel_Barbosa\dados\Contagem de Pantas Atacadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documents\Data Science\FitoData\Projetos\FitoData_Dan-B\dados\Contagem de Pantas Atacadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C90A475-C6A2-425F-8F6E-D7534C38FBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ACCEA2-1E32-4042-B153-E68D86534D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Incidência" sheetId="1" r:id="rId1"/>
+    <sheet name="Sobrevivência" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Incidência!$A$1:$I$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sobrevivência!$G$2:$J$82</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="17">
   <si>
     <t>Adjuvante</t>
   </si>
@@ -68,12 +70,24 @@
   <si>
     <t>Tratamento</t>
   </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>Contagem</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>número linhas</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,13 +113,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -135,6 +168,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -354,15 +405,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="3" max="9" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.88671875" customWidth="1"/>
     <col min="10" max="10" width="8.6640625" customWidth="1"/>
     <col min="11" max="11" width="10.77734375" customWidth="1"/>
     <col min="12" max="27" width="8.6640625" customWidth="1"/>
@@ -1456,31 +1511,31 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
+      <c r="A38" s="8">
         <v>10</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="9">
         <v>120</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="9">
         <v>1</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="9">
         <v>2</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="9">
         <v>4</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="9">
         <v>7</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="9">
         <v>4</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="9">
         <v>5</v>
       </c>
     </row>
@@ -11394,4 +11449,1314 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555FD7FC-3FCE-44A3-A5BC-9C7B65035B47}">
+  <dimension ref="A2:S82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="7"/>
+    <col min="4" max="4" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>10</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="5">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="G7" s="8">
+        <v>10</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G8" s="5">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G9" s="5">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G10" s="5">
+        <v>10</v>
+      </c>
+      <c r="H10" s="3">
+        <v>4</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
+      <c r="J10" s="3">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G11" s="8">
+        <v>10</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>7</v>
+      </c>
+      <c r="J11" s="9">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G12" s="5">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>7</v>
+      </c>
+      <c r="J12" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G13" s="5">
+        <v>10</v>
+      </c>
+      <c r="H13" s="3">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1">
+        <v>7</v>
+      </c>
+      <c r="J13" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G14" s="5">
+        <v>10</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4</v>
+      </c>
+      <c r="I14" s="1">
+        <v>7</v>
+      </c>
+      <c r="J14" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G15" s="8">
+        <v>10</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>10</v>
+      </c>
+      <c r="J15" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G16" s="5">
+        <v>10</v>
+      </c>
+      <c r="H16" s="3">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1">
+        <v>10</v>
+      </c>
+      <c r="J16" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+    </row>
+    <row r="17" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G17" s="5">
+        <v>10</v>
+      </c>
+      <c r="H17" s="3">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>10</v>
+      </c>
+      <c r="J17" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+    </row>
+    <row r="18" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G18" s="5">
+        <v>10</v>
+      </c>
+      <c r="H18" s="3">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>10</v>
+      </c>
+      <c r="J18" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+    </row>
+    <row r="19" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G19" s="8">
+        <v>10</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>17</v>
+      </c>
+      <c r="J19" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+    </row>
+    <row r="20" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G20" s="5">
+        <v>10</v>
+      </c>
+      <c r="H20" s="3">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1">
+        <v>17</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+    </row>
+    <row r="21" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G21" s="5">
+        <v>10</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3</v>
+      </c>
+      <c r="I21" s="1">
+        <v>17</v>
+      </c>
+      <c r="J21" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+    </row>
+    <row r="22" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G22" s="5">
+        <v>10</v>
+      </c>
+      <c r="H22" s="3">
+        <v>4</v>
+      </c>
+      <c r="I22" s="1">
+        <v>17</v>
+      </c>
+      <c r="J22" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+    </row>
+    <row r="23" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G23" s="5">
+        <v>11</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+    </row>
+    <row r="24" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G24" s="5">
+        <v>11</v>
+      </c>
+      <c r="H24" s="3">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+    </row>
+    <row r="25" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G25" s="5">
+        <v>11</v>
+      </c>
+      <c r="H25" s="3">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+    </row>
+    <row r="26" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G26" s="5">
+        <v>11</v>
+      </c>
+      <c r="H26" s="3">
+        <v>4</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G27" s="5">
+        <v>11</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>3</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G28" s="5">
+        <v>11</v>
+      </c>
+      <c r="H28" s="3">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1">
+        <v>3</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G29" s="5">
+        <v>11</v>
+      </c>
+      <c r="H29" s="3">
+        <v>3</v>
+      </c>
+      <c r="I29" s="1">
+        <v>3</v>
+      </c>
+      <c r="J29" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G30" s="5">
+        <v>11</v>
+      </c>
+      <c r="H30" s="3">
+        <v>4</v>
+      </c>
+      <c r="I30" s="1">
+        <v>3</v>
+      </c>
+      <c r="J30" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G31" s="5">
+        <v>11</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>7</v>
+      </c>
+      <c r="J31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="7:19" x14ac:dyDescent="0.3">
+      <c r="G32" s="5">
+        <v>11</v>
+      </c>
+      <c r="H32" s="3">
+        <v>2</v>
+      </c>
+      <c r="I32" s="1">
+        <v>7</v>
+      </c>
+      <c r="J32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G33" s="5">
+        <v>11</v>
+      </c>
+      <c r="H33" s="3">
+        <v>3</v>
+      </c>
+      <c r="I33" s="1">
+        <v>7</v>
+      </c>
+      <c r="J33" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G34" s="5">
+        <v>11</v>
+      </c>
+      <c r="H34" s="3">
+        <v>4</v>
+      </c>
+      <c r="I34" s="1">
+        <v>7</v>
+      </c>
+      <c r="J34" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G35" s="5">
+        <v>11</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>10</v>
+      </c>
+      <c r="J35" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G36" s="5">
+        <v>11</v>
+      </c>
+      <c r="H36" s="3">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1">
+        <v>10</v>
+      </c>
+      <c r="J36" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G37" s="5">
+        <v>11</v>
+      </c>
+      <c r="H37" s="3">
+        <v>3</v>
+      </c>
+      <c r="I37" s="1">
+        <v>10</v>
+      </c>
+      <c r="J37" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G38" s="5">
+        <v>11</v>
+      </c>
+      <c r="H38" s="3">
+        <v>4</v>
+      </c>
+      <c r="I38" s="1">
+        <v>10</v>
+      </c>
+      <c r="J38" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G39" s="5">
+        <v>11</v>
+      </c>
+      <c r="H39" s="3">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1">
+        <v>17</v>
+      </c>
+      <c r="J39" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G40" s="5">
+        <v>11</v>
+      </c>
+      <c r="H40" s="3">
+        <v>2</v>
+      </c>
+      <c r="I40" s="1">
+        <v>17</v>
+      </c>
+      <c r="J40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G41" s="5">
+        <v>11</v>
+      </c>
+      <c r="H41" s="3">
+        <v>3</v>
+      </c>
+      <c r="I41" s="1">
+        <v>17</v>
+      </c>
+      <c r="J41" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G42" s="5">
+        <v>11</v>
+      </c>
+      <c r="H42" s="3">
+        <v>4</v>
+      </c>
+      <c r="I42" s="1">
+        <v>17</v>
+      </c>
+      <c r="J42" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G43" s="5">
+        <v>12</v>
+      </c>
+      <c r="H43" s="3">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0</v>
+      </c>
+      <c r="J43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G44" s="5">
+        <v>12</v>
+      </c>
+      <c r="H44" s="3">
+        <v>2</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="J44" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G45" s="5">
+        <v>12</v>
+      </c>
+      <c r="H45" s="3">
+        <v>3</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G46" s="5">
+        <v>12</v>
+      </c>
+      <c r="H46" s="3">
+        <v>4</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+      <c r="J46" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G47" s="5">
+        <v>12</v>
+      </c>
+      <c r="H47" s="3">
+        <v>1</v>
+      </c>
+      <c r="I47" s="1">
+        <v>3</v>
+      </c>
+      <c r="J47" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G48" s="5">
+        <v>12</v>
+      </c>
+      <c r="H48" s="3">
+        <v>2</v>
+      </c>
+      <c r="I48" s="1">
+        <v>3</v>
+      </c>
+      <c r="J48" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G49" s="5">
+        <v>12</v>
+      </c>
+      <c r="H49" s="3">
+        <v>3</v>
+      </c>
+      <c r="I49" s="1">
+        <v>3</v>
+      </c>
+      <c r="J49" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G50" s="5">
+        <v>12</v>
+      </c>
+      <c r="H50" s="3">
+        <v>4</v>
+      </c>
+      <c r="I50" s="1">
+        <v>3</v>
+      </c>
+      <c r="J50" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G51" s="5">
+        <v>12</v>
+      </c>
+      <c r="H51" s="3">
+        <v>1</v>
+      </c>
+      <c r="I51" s="1">
+        <v>7</v>
+      </c>
+      <c r="J51" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G52" s="5">
+        <v>12</v>
+      </c>
+      <c r="H52" s="3">
+        <v>2</v>
+      </c>
+      <c r="I52" s="1">
+        <v>7</v>
+      </c>
+      <c r="J52" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G53" s="5">
+        <v>12</v>
+      </c>
+      <c r="H53" s="3">
+        <v>3</v>
+      </c>
+      <c r="I53" s="1">
+        <v>7</v>
+      </c>
+      <c r="J53" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G54" s="5">
+        <v>12</v>
+      </c>
+      <c r="H54" s="3">
+        <v>4</v>
+      </c>
+      <c r="I54" s="1">
+        <v>7</v>
+      </c>
+      <c r="J54" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G55" s="5">
+        <v>12</v>
+      </c>
+      <c r="H55" s="3">
+        <v>1</v>
+      </c>
+      <c r="I55" s="1">
+        <v>10</v>
+      </c>
+      <c r="J55" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G56" s="5">
+        <v>12</v>
+      </c>
+      <c r="H56" s="3">
+        <v>2</v>
+      </c>
+      <c r="I56" s="1">
+        <v>10</v>
+      </c>
+      <c r="J56" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G57" s="5">
+        <v>12</v>
+      </c>
+      <c r="H57" s="3">
+        <v>3</v>
+      </c>
+      <c r="I57" s="1">
+        <v>10</v>
+      </c>
+      <c r="J57" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G58" s="5">
+        <v>12</v>
+      </c>
+      <c r="H58" s="3">
+        <v>4</v>
+      </c>
+      <c r="I58" s="1">
+        <v>10</v>
+      </c>
+      <c r="J58" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G59" s="5">
+        <v>12</v>
+      </c>
+      <c r="H59" s="3">
+        <v>1</v>
+      </c>
+      <c r="I59" s="1">
+        <v>17</v>
+      </c>
+      <c r="J59" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G60" s="5">
+        <v>12</v>
+      </c>
+      <c r="H60" s="3">
+        <v>2</v>
+      </c>
+      <c r="I60" s="1">
+        <v>17</v>
+      </c>
+      <c r="J60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G61" s="5">
+        <v>12</v>
+      </c>
+      <c r="H61" s="3">
+        <v>3</v>
+      </c>
+      <c r="I61" s="1">
+        <v>17</v>
+      </c>
+      <c r="J61" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G62" s="5">
+        <v>12</v>
+      </c>
+      <c r="H62" s="3">
+        <v>4</v>
+      </c>
+      <c r="I62" s="1">
+        <v>17</v>
+      </c>
+      <c r="J62" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G63" s="5">
+        <v>13</v>
+      </c>
+      <c r="H63" s="3">
+        <v>1</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0</v>
+      </c>
+      <c r="J63" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G64" s="5">
+        <v>13</v>
+      </c>
+      <c r="H64" s="3">
+        <v>2</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G65" s="5">
+        <v>13</v>
+      </c>
+      <c r="H65" s="3">
+        <v>3</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0</v>
+      </c>
+      <c r="J65" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G66" s="5">
+        <v>13</v>
+      </c>
+      <c r="H66" s="3">
+        <v>4</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0</v>
+      </c>
+      <c r="J66" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G67" s="5">
+        <v>13</v>
+      </c>
+      <c r="H67" s="3">
+        <v>1</v>
+      </c>
+      <c r="I67" s="1">
+        <v>3</v>
+      </c>
+      <c r="J67" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G68" s="5">
+        <v>13</v>
+      </c>
+      <c r="H68" s="3">
+        <v>2</v>
+      </c>
+      <c r="I68" s="1">
+        <v>3</v>
+      </c>
+      <c r="J68" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G69" s="5">
+        <v>13</v>
+      </c>
+      <c r="H69" s="3">
+        <v>3</v>
+      </c>
+      <c r="I69" s="1">
+        <v>3</v>
+      </c>
+      <c r="J69" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G70" s="5">
+        <v>13</v>
+      </c>
+      <c r="H70" s="3">
+        <v>4</v>
+      </c>
+      <c r="I70" s="1">
+        <v>3</v>
+      </c>
+      <c r="J70" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G71" s="5">
+        <v>13</v>
+      </c>
+      <c r="H71" s="3">
+        <v>1</v>
+      </c>
+      <c r="I71" s="1">
+        <v>7</v>
+      </c>
+      <c r="J71" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G72" s="5">
+        <v>13</v>
+      </c>
+      <c r="H72" s="3">
+        <v>2</v>
+      </c>
+      <c r="I72" s="1">
+        <v>7</v>
+      </c>
+      <c r="J72" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G73" s="5">
+        <v>13</v>
+      </c>
+      <c r="H73" s="3">
+        <v>3</v>
+      </c>
+      <c r="I73" s="1">
+        <v>7</v>
+      </c>
+      <c r="J73" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G74" s="5">
+        <v>13</v>
+      </c>
+      <c r="H74" s="3">
+        <v>4</v>
+      </c>
+      <c r="I74" s="1">
+        <v>7</v>
+      </c>
+      <c r="J74" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G75" s="5">
+        <v>13</v>
+      </c>
+      <c r="H75" s="3">
+        <v>1</v>
+      </c>
+      <c r="I75" s="1">
+        <v>10</v>
+      </c>
+      <c r="J75" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G76" s="5">
+        <v>13</v>
+      </c>
+      <c r="H76" s="3">
+        <v>2</v>
+      </c>
+      <c r="I76" s="1">
+        <v>10</v>
+      </c>
+      <c r="J76" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G77" s="5">
+        <v>13</v>
+      </c>
+      <c r="H77" s="3">
+        <v>3</v>
+      </c>
+      <c r="I77" s="1">
+        <v>10</v>
+      </c>
+      <c r="J77" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G78" s="5">
+        <v>13</v>
+      </c>
+      <c r="H78" s="3">
+        <v>4</v>
+      </c>
+      <c r="I78" s="1">
+        <v>10</v>
+      </c>
+      <c r="J78" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G79" s="5">
+        <v>13</v>
+      </c>
+      <c r="H79" s="3">
+        <v>1</v>
+      </c>
+      <c r="I79" s="1">
+        <v>17</v>
+      </c>
+      <c r="J79" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G80" s="5">
+        <v>13</v>
+      </c>
+      <c r="H80" s="3">
+        <v>2</v>
+      </c>
+      <c r="I80" s="1">
+        <v>17</v>
+      </c>
+      <c r="J80" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G81" s="5">
+        <v>13</v>
+      </c>
+      <c r="H81" s="3">
+        <v>3</v>
+      </c>
+      <c r="I81" s="1">
+        <v>17</v>
+      </c>
+      <c r="J81" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G82" s="5">
+        <v>13</v>
+      </c>
+      <c r="H82" s="3">
+        <v>4</v>
+      </c>
+      <c r="I82" s="1">
+        <v>17</v>
+      </c>
+      <c r="J82" s="3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="G2:J82" xr:uid="{555FD7FC-3FCE-44A3-A5BC-9C7B65035B47}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G3:J82">
+      <sortCondition ref="G2:G82"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>